<commit_message>
Update with current changes.
</commit_message>
<xml_diff>
--- a/AISProcessing_V2_ChangeList.xlsx
+++ b/AISProcessing_V2_ChangeList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/kapsarke_msu_edu/Documents/Sync/AISProcessing_V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{28E13EBF-43B2-44E7-BCD9-9EEA59FF4CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E780F2A0-CBC2-496A-94CB-C08E5DCD2936}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{28E13EBF-43B2-44E7-BCD9-9EEA59FF4CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDB6335A-591C-4664-BEE0-5DB019A94127}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3772F258-5377-4D47-8A32-1FFA9CEE7FF9}"/>
+    <workbookView xWindow="-25320" yWindow="465" windowWidth="25440" windowHeight="15390" xr2:uid="{3772F258-5377-4D47-8A32-1FFA9CEE7FF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Issue/Update</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Complete?</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +559,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
@@ -568,7 +573,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -578,7 +585,9 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
@@ -588,7 +597,9 @@
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -600,7 +611,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -612,7 +625,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
@@ -624,7 +639,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Update to reflect latest changes to scripts.
</commit_message>
<xml_diff>
--- a/AISProcessing_V2_ChangeList.xlsx
+++ b/AISProcessing_V2_ChangeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/kapsarke_msu_edu/Documents/Sync/AISProcessing_V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{28E13EBF-43B2-44E7-BCD9-9EEA59FF4CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDB6335A-591C-4664-BEE0-5DB019A94127}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{28E13EBF-43B2-44E7-BCD9-9EEA59FF4CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D22A3404-BB74-48F9-828B-1E5228C5F934}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="465" windowWidth="25440" windowHeight="15390" xr2:uid="{3772F258-5377-4D47-8A32-1FFA9CEE7FF9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Issue/Update</t>
   </si>
@@ -128,6 +128,24 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Add spoof remover into vectorization script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ended up not needing it because I implemented a 60 km limit between successive points. </t>
+  </si>
+  <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEED TO TEST WHETHER THIS LIMIT BIASES THE DATA IN EARLY YEARS WITH LESS SATELLITE COVERAGE… </t>
+  </si>
+  <si>
+    <t>Improved ship type assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instead of just taking the metadata from the first static message transmitted for each ship each day, the new script takes the most frequently transmitted ship type in all static messages for each ship in each month (downweighting NA and 0 entries). This minimizes the overall chance of error. Also, the new script assigns static information from vessels to transit segments based on monthly transmissions rather than daily (AISlookup is joined to AISsf based on MMSI, not AIS_ID). </t>
   </si>
 </sst>
 </file>
@@ -197,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +232,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,22 +550,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E1362C-434B-4328-9A44-160CF2C2666A}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" customWidth="1"/>
     <col min="4" max="4" width="105.140625" customWidth="1"/>
     <col min="5" max="5" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -558,7 +579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -572,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -584,7 +605,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -596,7 +617,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -610,7 +631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -624,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -638,7 +659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -652,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -664,8 +685,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -676,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
@@ -688,7 +711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -700,25 +723,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="5"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>